<commit_message>
docs(reports): Week 1 update
</commit_message>
<xml_diff>
--- a/documentos/organización/Cronograma_LuisMellado.xlsx
+++ b/documentos/organización/Cronograma_LuisMellado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mella\OneDrive\Escritorio\TFG_LuisMellado_JoseMar-aMoyano\documentos\organización\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ACBFF1-D8A8-457D-9D5A-A4D3FEB78B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DEB0E1-220B-45E3-95CF-231C5398722C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,7 +228,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +250,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -396,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -480,6 +492,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -768,7 +792,7 @@
   <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -898,13 +922,13 @@
       <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17">
-        <v>1</v>
-      </c>
-      <c r="D3" s="17">
-        <v>1</v>
-      </c>
-      <c r="E3" s="17">
+      <c r="C3" s="29">
+        <v>1</v>
+      </c>
+      <c r="D3" s="29">
+        <v>1</v>
+      </c>
+      <c r="E3" s="29">
         <v>1</v>
       </c>
       <c r="F3" s="18"/>
@@ -943,7 +967,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="21">
+      <c r="E4" s="31">
         <v>1</v>
       </c>
       <c r="F4" s="22"/>
@@ -987,7 +1011,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
-      <c r="H5" s="21">
+      <c r="H5" s="31">
         <v>1</v>
       </c>
       <c r="I5" s="21">
@@ -1030,10 +1054,10 @@
       <c r="G6" s="22"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="21">
-        <v>1</v>
-      </c>
-      <c r="K6" s="21">
+      <c r="J6" s="30">
+        <v>1</v>
+      </c>
+      <c r="K6" s="30">
         <v>1</v>
       </c>
       <c r="L6" s="21">
@@ -1133,7 +1157,7 @@
       <c r="F8" s="24"/>
       <c r="G8" s="24"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="25">
+      <c r="I8" s="32">
         <v>1</v>
       </c>
       <c r="J8" s="25">

</xml_diff>

<commit_message>
docs(reports): Week 2 update
</commit_message>
<xml_diff>
--- a/documentos/organización/Cronograma_LuisMellado.xlsx
+++ b/documentos/organización/Cronograma_LuisMellado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mella\OneDrive\Escritorio\TFG_LuisMellado_JoseMar-aMoyano\documentos\organización\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosan\Desktop\TFG_LuisMellado_JoseMar-aMoyano\documentos\organización\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DEB0E1-220B-45E3-95CF-231C5398722C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78012F5-BDAB-4DEE-916D-38F42D5ADA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -458,9 +458,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -491,19 +488,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -792,32 +792,32 @@
   <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.453125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="7.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="12"/>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="28"/>
+      <c r="G1" s="30"/>
       <c r="V1" s="13" t="s">
         <v>7</v>
       </c>
@@ -828,7 +828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -914,7 +914,7 @@
         <v>45438</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <f t="shared" ref="A3:A8" si="0">ROUND(SUMPRODUCT(C3:AB3,C$9:AB$9),2)</f>
         <v>2.83</v>
@@ -922,21 +922,21 @@
       <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="29">
-        <v>1</v>
-      </c>
-      <c r="D3" s="29">
-        <v>1</v>
-      </c>
-      <c r="E3" s="29">
-        <v>1</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="17">
-        <v>1</v>
-      </c>
-      <c r="I3" s="19"/>
+      <c r="C3" s="27">
+        <v>1</v>
+      </c>
+      <c r="D3" s="27">
+        <v>1</v>
+      </c>
+      <c r="E3" s="27">
+        <v>1</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="32">
+        <v>1</v>
+      </c>
+      <c r="I3" s="18"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -949,15 +949,15 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
-      <c r="V3" s="18"/>
+      <c r="V3" s="17"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
-      <c r="Y3" s="18"/>
+      <c r="Y3" s="17"/>
       <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
-      <c r="AB3" s="20"/>
+      <c r="AB3" s="19"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <f t="shared" si="0"/>
         <v>1.17</v>
@@ -967,15 +967,15 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="31">
-        <v>1</v>
-      </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="21">
-        <v>1</v>
-      </c>
-      <c r="I4" s="21">
+      <c r="E4" s="29">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="20">
+        <v>1</v>
+      </c>
+      <c r="I4" s="20">
         <v>1</v>
       </c>
       <c r="J4" s="5"/>
@@ -990,15 +990,15 @@
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
-      <c r="V4" s="22"/>
+      <c r="V4" s="21"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
-      <c r="Y4" s="22"/>
+      <c r="Y4" s="21"/>
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
-      <c r="AB4" s="23"/>
+      <c r="AB4" s="22"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1009,15 +1009,15 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="31">
-        <v>1</v>
-      </c>
-      <c r="I5" s="21">
-        <v>1</v>
-      </c>
-      <c r="J5" s="21">
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="29">
+        <v>1</v>
+      </c>
+      <c r="I5" s="20">
+        <v>1</v>
+      </c>
+      <c r="J5" s="20">
         <v>1</v>
       </c>
       <c r="K5" s="5"/>
@@ -1031,15 +1031,15 @@
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
-      <c r="V5" s="22"/>
+      <c r="V5" s="21"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
-      <c r="Y5" s="22"/>
+      <c r="Y5" s="21"/>
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
-      <c r="AB5" s="23"/>
+      <c r="AB5" s="22"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <f t="shared" si="0"/>
         <v>7.33</v>
@@ -1050,51 +1050,51 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="30">
-        <v>1</v>
-      </c>
-      <c r="K6" s="30">
-        <v>1</v>
-      </c>
-      <c r="L6" s="21">
-        <v>1</v>
-      </c>
-      <c r="M6" s="21">
-        <v>1</v>
-      </c>
-      <c r="N6" s="21">
-        <v>1</v>
-      </c>
-      <c r="O6" s="21">
-        <v>1</v>
-      </c>
-      <c r="P6" s="21">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="21">
-        <v>1</v>
-      </c>
-      <c r="R6" s="21">
-        <v>1</v>
-      </c>
-      <c r="S6" s="21">
+      <c r="J6" s="28">
+        <v>1</v>
+      </c>
+      <c r="K6" s="28">
+        <v>1</v>
+      </c>
+      <c r="L6" s="28">
+        <v>1</v>
+      </c>
+      <c r="M6" s="20">
+        <v>1</v>
+      </c>
+      <c r="N6" s="20">
+        <v>1</v>
+      </c>
+      <c r="O6" s="20">
+        <v>1</v>
+      </c>
+      <c r="P6" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>1</v>
+      </c>
+      <c r="R6" s="20">
+        <v>1</v>
+      </c>
+      <c r="S6" s="20">
         <v>1</v>
       </c>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
-      <c r="V6" s="22"/>
+      <c r="V6" s="21"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
-      <c r="Y6" s="22"/>
+      <c r="Y6" s="21"/>
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
-      <c r="AB6" s="23"/>
+      <c r="AB6" s="22"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <f t="shared" si="0"/>
         <v>3.5</v>
@@ -1105,8 +1105,8 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -1116,34 +1116,34 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="21">
-        <v>1</v>
-      </c>
-      <c r="R7" s="21">
-        <v>1</v>
-      </c>
-      <c r="S7" s="21">
-        <v>1</v>
-      </c>
-      <c r="T7" s="21">
-        <v>1</v>
-      </c>
-      <c r="U7" s="21">
-        <v>1</v>
-      </c>
-      <c r="V7" s="22"/>
-      <c r="W7" s="21">
-        <v>1</v>
-      </c>
-      <c r="X7" s="21">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="22"/>
+      <c r="Q7" s="20">
+        <v>1</v>
+      </c>
+      <c r="R7" s="20">
+        <v>1</v>
+      </c>
+      <c r="S7" s="20">
+        <v>1</v>
+      </c>
+      <c r="T7" s="20">
+        <v>1</v>
+      </c>
+      <c r="U7" s="20">
+        <v>1</v>
+      </c>
+      <c r="V7" s="21"/>
+      <c r="W7" s="20">
+        <v>1</v>
+      </c>
+      <c r="X7" s="20">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="21"/>
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
-      <c r="AB7" s="23"/>
+      <c r="AB7" s="22"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>5.17</v>
@@ -1154,16 +1154,16 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="32">
-        <v>1</v>
-      </c>
-      <c r="J8" s="25">
-        <v>1</v>
-      </c>
-      <c r="K8" s="25">
+      <c r="I8" s="31">
+        <v>1</v>
+      </c>
+      <c r="J8" s="31">
+        <v>1</v>
+      </c>
+      <c r="K8" s="24">
         <v>1</v>
       </c>
       <c r="L8" s="2"/>
@@ -1174,29 +1174,29 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
-      <c r="T8" s="25">
-        <v>1</v>
-      </c>
-      <c r="U8" s="25">
-        <v>1</v>
-      </c>
-      <c r="V8" s="24"/>
-      <c r="W8" s="25">
-        <v>1</v>
-      </c>
-      <c r="X8" s="25">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="25">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="25">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="26"/>
+      <c r="T8" s="24">
+        <v>1</v>
+      </c>
+      <c r="U8" s="24">
+        <v>1</v>
+      </c>
+      <c r="V8" s="23"/>
+      <c r="W8" s="24">
+        <v>1</v>
+      </c>
+      <c r="X8" s="24">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="24">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="24">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="25"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <f>SUM(A3:A8)</f>
         <v>21</v>
@@ -1213,8 +1213,8 @@
         <f t="shared" ref="E9:AB9" si="2">IF(SUM(E3:E8)=0,0,1/SUM(E3:E8))</f>
         <v>0.5</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="1">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
@@ -1271,7 +1271,7 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="V9" s="27"/>
+      <c r="V9" s="26"/>
       <c r="W9" s="1">
         <f t="shared" si="2"/>
         <v>0.5</v>
@@ -1280,7 +1280,7 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="Y9" s="27"/>
+      <c r="Y9" s="26"/>
       <c r="Z9" s="1">
         <f t="shared" si="2"/>
         <v>1</v>

</xml_diff>